<commit_message>
Hard works - add students
</commit_message>
<xml_diff>
--- a/ИТиП_FullReport_УК-2971.xlsx
+++ b/ИТиП_FullReport_УК-2971.xlsx
@@ -90,14 +90,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BDECB6"/>
-        <bgColor rgb="00BDECB6"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="00BDECB6"/>
+        <bgColor rgb="00BDECB6"/>
       </patternFill>
     </fill>
   </fills>
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,7 +423,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,169 +442,201 @@
       <c r="F1" s="1" t="n">
         <v>45637</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="n">
+        <v>45637</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>45637</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="n"/>
-    </row>
-    <row r="3" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="2" t="n"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="n"/>
-    </row>
-    <row r="4" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="2" t="n"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="3" t="n"/>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-    </row>
-    <row r="5" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="3" t="n"/>
+      <c r="F4" s="3" t="n"/>
+      <c r="G4" s="3" t="n"/>
+      <c r="H4" s="2" t="n"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="n"/>
-      <c r="D5" s="3" t="n"/>
-      <c r="E5" s="2" t="n"/>
-      <c r="F5" s="2" t="n"/>
-    </row>
-    <row r="6" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
+      <c r="H5" s="2" t="n"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="2" t="n"/>
-      <c r="F6" s="2" t="n"/>
-    </row>
-    <row r="7" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="3" t="n"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="2" t="n"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="3" t="n"/>
-      <c r="E7" s="2" t="n"/>
-      <c r="F7" s="2" t="n"/>
-    </row>
-    <row r="8" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="2" t="n"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="3" t="n"/>
-      <c r="E8" s="2" t="n"/>
-      <c r="F8" s="2" t="n"/>
-    </row>
-    <row r="9" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="3" t="n"/>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="2" t="n"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" s="2" t="n"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="B9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="3" t="n"/>
+      <c r="F9" s="2" t="n"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="3" t="n"/>
-      <c r="E10" s="2" t="n"/>
-      <c r="F10" s="2" t="n"/>
-    </row>
-    <row r="11" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="3" t="n"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
+      <c r="H10" s="2" t="n"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="n"/>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="2" t="n"/>
-      <c r="F11" s="2" t="n"/>
-    </row>
-    <row r="12" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="3" t="n"/>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="2" t="n"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="3" t="n"/>
-      <c r="E12" s="2" t="n"/>
-      <c r="F12" s="2" t="n"/>
-    </row>
-    <row r="13" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="3" t="n"/>
+      <c r="F12" s="3" t="n"/>
+      <c r="G12" s="3" t="n"/>
+      <c r="H12" s="2" t="n"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="n"/>
-      <c r="D13" s="3" t="n"/>
-      <c r="E13" s="2" t="n"/>
-      <c r="F13" s="2" t="n"/>
-    </row>
-    <row r="14" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="3" t="n"/>
+      <c r="F13" s="3" t="n"/>
+      <c r="G13" s="3" t="n"/>
+      <c r="H13" s="2" t="n"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="n"/>
-      <c r="D14" s="3" t="n"/>
-      <c r="E14" s="2" t="n"/>
-      <c r="F14" s="2" t="n"/>
-    </row>
-    <row r="16" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="3" t="n"/>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
+      <c r="H14" s="2" t="n"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8">
       <c r="A17" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>